<commit_message>
stort arbete på Level1, samt uppdaterat personliga filer
:abcd:
</commit_message>
<xml_diff>
--- a/Documents/Personal files/TL/TidsrapportVecka16Tim.xlsx
+++ b/Documents/Personal files/TL/TidsrapportVecka16Tim.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Tidsrapport</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>2015-04-13 - 2015-04-19</t>
+  </si>
+  <si>
+    <t>Puzzeldesign och nivådesign</t>
+  </si>
+  <si>
+    <t>nivådesign</t>
   </si>
 </sst>
 </file>
@@ -157,35 +163,19 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -195,6 +185,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,151 +505,168 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4"/>
+      <c r="B3" s="13">
+        <v>16</v>
+      </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>42086</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="5">
+        <v>42107</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13">
+      <c r="C9" s="15"/>
+      <c r="D9" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>42087</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13">
+      <c r="A10" s="5">
+        <v>42108</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>42088</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13">
+      <c r="A11" s="5">
+        <v>42109</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
-        <v>42089</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="5">
+        <v>42110</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>42090</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="5">
+        <v>42111</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>42091</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="5">
+        <v>42112</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>42092</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
+      <c r="A15" s="5">
+        <v>42113</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="10">
         <f>D9+D10+D11+D12+D13+D14+D15</f>
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -656,12 +679,12 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>